<commit_message>
Updated Class and Race special abilities
</commit_message>
<xml_diff>
--- a/Sunken Temple/Sunken Temple.xlsx
+++ b/Sunken Temple/Sunken Temple.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
   <si>
     <t>Dwarf</t>
   </si>
@@ -99,15 +99,9 @@
     <t>Strength</t>
   </si>
   <si>
-    <t>.+3 Attack Power</t>
-  </si>
-  <si>
     <t>Explode</t>
   </si>
   <si>
-    <t>One-shots are double damage</t>
-  </si>
-  <si>
     <t>Penalty</t>
   </si>
   <si>
@@ -123,12 +117,6 @@
     <t>Resistant to all Magic attacks</t>
   </si>
   <si>
-    <t>Collector</t>
-  </si>
-  <si>
-    <t>.+4 unequipped items</t>
-  </si>
-  <si>
     <t>Summon</t>
   </si>
   <si>
@@ -181,13 +169,88 @@
   </si>
   <si>
     <t>.+4 Attack Power</t>
+  </si>
+  <si>
+    <t>Volcanic Pressure</t>
+  </si>
+  <si>
+    <t>Ability to make a diamond when 1 of each color gemstone is combined</t>
+  </si>
+  <si>
+    <t>.x2 the gemstones when receiving them from a chest</t>
+  </si>
+  <si>
+    <t>Gem Finder</t>
+  </si>
+  <si>
+    <t>.+ 1 to Attack Power, +1 to Escape</t>
+  </si>
+  <si>
+    <t>First Strike</t>
+  </si>
+  <si>
+    <t>Emotionless, you do not hesistate. If you are beating a monster at the beggining of a battle you can terminate it immediately. No one can interfer. Monsters can still try to run. (cannot be used to win)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For a price (insert here) you can see into the future. This includes, the ability to know what type a temple guardian is and whether or not a chest is good or bad. </t>
+  </si>
+  <si>
+    <t>Hidden Blade</t>
+  </si>
+  <si>
+    <t>Theft</t>
+  </si>
+  <si>
+    <t>Stealth</t>
+  </si>
+  <si>
+    <t>.+2 to Escape</t>
+  </si>
+  <si>
+    <t>Master of Disguise</t>
+  </si>
+  <si>
+    <t>Prophetic</t>
+  </si>
+  <si>
+    <t>Foresight</t>
+  </si>
+  <si>
+    <t>Cannot be surprised. (insert here)</t>
+  </si>
+  <si>
+    <t>.+3 Attack Power per monster</t>
+  </si>
+  <si>
+    <t>In tune with Nature</t>
+  </si>
+  <si>
+    <t>Agile</t>
+  </si>
+  <si>
+    <t>.+2 attack Power</t>
+  </si>
+  <si>
+    <t>One-shots are worth double</t>
+  </si>
+  <si>
+    <t>Sacrifice</t>
+  </si>
+  <si>
+    <t>Fire Ball</t>
+  </si>
+  <si>
+    <t>Lightning Bolt</t>
+  </si>
+  <si>
+    <t>Icy Touch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,6 +272,11 @@
       <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -268,7 +336,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -330,8 +398,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -377,8 +456,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -405,6 +492,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -412,40 +520,37 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -468,6 +573,10 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -490,6 +599,10 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -819,17 +932,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J42"/>
+  <dimension ref="C3:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
@@ -956,15 +1070,15 @@
       <c r="H11" s="5"/>
       <c r="I11" s="6"/>
       <c r="J11" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="3:10">
-      <c r="D12" s="16"/>
+      <c r="D12" s="11"/>
     </row>
     <row r="14" spans="3:10">
-      <c r="C14" s="22" t="s">
-        <v>40</v>
+      <c r="C14" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>18</v>
@@ -972,331 +1086,403 @@
       <c r="E14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="14" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10">
+      <c r="C15" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="3:10">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="C17" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="C19" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="3:7">
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="3:7">
+      <c r="C22" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="3:7">
+      <c r="C23" s="24"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="3:7">
+      <c r="C24" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="3:10">
-      <c r="C15" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="18" t="s">
+      <c r="F24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="3:7">
+      <c r="C25" s="24"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="3:7">
+      <c r="C26" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="3:10">
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="3:7">
-      <c r="C17" s="10" t="s">
+      <c r="D26" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="3:7">
+      <c r="C27" s="24"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="3:7">
+      <c r="C28" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="3:7" ht="45">
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="3:7">
+      <c r="C30" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="3:7">
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="3:7">
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="3:7">
+      <c r="C33" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="3:7">
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="3:7">
+      <c r="C35" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="3:7">
+      <c r="C36" s="20"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="10"/>
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="3:7">
+      <c r="C37" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="3:7">
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="3:7">
+      <c r="C39" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="3:7">
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="3:7">
-      <c r="C19" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="3:7">
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="3:7">
-      <c r="C21" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="3:7">
-      <c r="C22" s="14"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="3:7">
-      <c r="C23" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="3:7">
-      <c r="C24" s="14"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="3:7">
-      <c r="C25" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="3:7">
-      <c r="C26" s="14"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="15"/>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="3:7">
-      <c r="C27" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="3:7">
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="3:7">
-      <c r="C29" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="3:7">
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="3:7">
-      <c r="C31" s="12" t="s">
+      <c r="D39" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="3:7" ht="45">
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="3:7">
+      <c r="C41" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" spans="3:7">
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" s="10"/>
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="3:7">
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F43" s="10"/>
+      <c r="G43" s="4"/>
+    </row>
+    <row r="44" spans="3:7">
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F44" s="10"/>
+      <c r="G44" s="4"/>
+    </row>
+    <row r="45" spans="3:7">
+      <c r="C45" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="3:7">
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="3:7">
-      <c r="C33" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="3:7">
-      <c r="C34" s="21"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F34" s="15"/>
-      <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="3:7">
-      <c r="C35" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="3:7">
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="4"/>
-    </row>
-    <row r="37" spans="3:7">
-      <c r="C37" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="4"/>
-    </row>
-    <row r="38" spans="3:7">
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="4"/>
-    </row>
-    <row r="39" spans="3:7">
-      <c r="C39" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="3:7">
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="4"/>
-    </row>
-    <row r="41" spans="3:7">
-      <c r="C41" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="12" t="s">
+      <c r="D45" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E45" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F41" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G41" s="4"/>
-    </row>
-    <row r="42" spans="3:7">
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="4"/>
+      <c r="F45" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G45" s="4"/>
+    </row>
+    <row r="46" spans="3:7">
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D41:D44"/>
+    <mergeCell ref="D37:D38"/>
     <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C44"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C32"/>
     <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D22:D23"/>
     <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D37:D38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>